<commit_message>
working on the paper
</commit_message>
<xml_diff>
--- a/scam17_revision.xlsx
+++ b/scam17_revision.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ScratchVars\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4440" activeTab="1"/>
+    <workbookView xWindow="51140" yWindow="0" windowWidth="28860" windowHeight="17040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rev1" sheetId="1" r:id="rId1"/>
     <sheet name="rev2" sheetId="2" r:id="rId2"/>
+    <sheet name="rev3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
   <si>
     <t>Using the term readability vs understandability</t>
   </si>
@@ -325,21 +324,120 @@
 I added to the story the research on difficulties faced by learners in Abstract/Related Work/Conclusion citing the Kolling et. al.</t>
   </si>
   <si>
-    <t>Fig. 7 shows the data for scratch projects. Comparison with the other PL languages is statistcally performed, but the original data itself is not presented in our paper. It is not clear to me what the reviewer means by supporting data here</t>
-  </si>
-  <si>
     <t xml:space="preserve">To Do: check </t>
   </si>
   <si>
     <t>To Do
 Change the graph by excluding the 11th item</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>Could it be novice programmers erfer longer names?</t>
+  </si>
+  <si>
+    <t>The reviewer essentially asks whether the phenomen we observe should be attributed to Scratch as a programming language or to the level of familiarity with programming as such.</t>
+  </si>
+  <si>
+    <t>Nice inclusion of implications</t>
+  </si>
+  <si>
+    <t>Indeed</t>
+  </si>
+  <si>
+    <t>None required</t>
+  </si>
+  <si>
+    <t>p.1</t>
+  </si>
+  <si>
+    <t>suggesting TO the learner</t>
+  </si>
+  <si>
+    <t>already fixed</t>
+  </si>
+  <si>
+    <t>p.2</t>
+  </si>
+  <si>
+    <t>Broken box</t>
+  </si>
+  <si>
+    <t>To be fixed</t>
+  </si>
+  <si>
+    <t>p.5</t>
+  </si>
+  <si>
+    <t>Add a full stop after [35]</t>
+  </si>
+  <si>
+    <t>Choice of newer stat. test well-justified</t>
+  </si>
+  <si>
+    <t>pp.6-7</t>
+  </si>
+  <si>
+    <t>Move Fig 8 (repetition blocks) to the previous page.</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>p.7</t>
+  </si>
+  <si>
+    <t>Expectations &amp; contradictions clearly stated to ease interpretations if results</t>
+  </si>
+  <si>
+    <t>Includes concrete examples to explain results</t>
+  </si>
+  <si>
+    <t>Figures out of order</t>
+  </si>
+  <si>
+    <t>We follow the order of Observations a)-c) not of figures</t>
+  </si>
+  <si>
+    <t>p.8</t>
+  </si>
+  <si>
+    <t>Would be really interesting to see for the other PLs!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.9 </t>
+  </si>
+  <si>
+    <t>Missing related work: But does this hold for other languages see Libelit in PPIG 2016 for Java</t>
+  </si>
+  <si>
+    <t>p.10</t>
+  </si>
+  <si>
+    <t>Perhaps other name analysis is also relevant, like Einar Host?</t>
+  </si>
+  <si>
+    <t>Fig. 7 shows the data for scratch projects. Comparison with the other PL languages is statistcally performed, but the original data itself is not presented in our paper. It is not clear to me what the reviewer means by supporting data here. Alexander: we state in V-A that in Scratch the single-letter variables constitute ca. 4%, while Beniamini et al. have observed 9-20%. I've added explicit percentages in the box.</t>
+  </si>
+  <si>
+    <t>Changed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right. This is a consequence of me being an idiot and mixing different distance metrics. </t>
+  </si>
+  <si>
+    <t>p &lt; 2.2*10^-16</t>
+  </si>
+  <si>
+    <t>Changed. "too small to be computed precisely"---floating point numbers underflow.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +478,22 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -432,8 +546,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -465,7 +583,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -552,7 +674,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,7 +709,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -764,7 +886,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -775,20 +897,20 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41" style="1" customWidth="1"/>
-    <col min="2" max="2" width="65.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="58" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="19.1640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -805,7 +927,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="110.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="110.25" customHeight="1" thickTop="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -822,7 +944,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="64">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -839,7 +961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="48">
       <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
@@ -856,7 +978,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="131.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="96">
       <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
@@ -873,7 +995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="64">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -888,7 +1010,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="48">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -905,7 +1027,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="112">
       <c r="A8" s="5" t="s">
         <v>51</v>
       </c>
@@ -920,7 +1042,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -928,7 +1050,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -936,21 +1063,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="55.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="55.5703125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="56.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="56.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="55.5" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -967,7 +1094,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="122.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="215" customHeight="1" thickTop="1">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -984,7 +1111,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="80">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -1001,7 +1128,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" ht="189.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="5" customFormat="1" ht="128">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
@@ -1009,13 +1136,13 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="5" customFormat="1" ht="128">
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
@@ -1026,13 +1153,13 @@
         <v>21</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="279.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="279.75" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -1047,7 +1174,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="5" customFormat="1" ht="64">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
@@ -1056,13 +1183,13 @@
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" ht="128">
       <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
@@ -1074,10 +1201,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="32">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -1091,10 +1218,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="32">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1111,7 +1238,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="128">
       <c r="A11" s="9" t="s">
         <v>30</v>
       </c>
@@ -1123,10 +1250,199 @@
         <v>45</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="76" customWidth="1"/>
+    <col min="3" max="3" width="57.83203125" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>